<commit_message>
feat: add cash purchase import and update PDF templates
- Add new cash purchase import interface (Import.jsx)
- Refactor CashPurchaseImport class for improved data handling
- Update cash purchase list with import functionality
- Fix balance sheet currency field (base_currency -> currency)
- Reformat all PDF templates for consistency:
  * invoice, cash-invoice, deferred-invoice
  * bill-invoice, bill-payment, receive-payment
  * cash-purchase, purchase-order, purchase-return
  * quotation, sales-return
- Update sample cash purchases Excel template
- Clean up code formatting in ReportController
</commit_message>
<xml_diff>
--- a/public/uploads/media/default/sample_cash_purchases.xlsx
+++ b/public/uploads/media/default/sample_cash_purchases.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahaf\Desktop\Mohamed\Sahafintech\ekstrabooks-v2.0\public\uploads\media\default\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahaf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7C1D5F-A7EC-49AA-AC97-5B329FF0AA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="sample_cash_invoices" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,29 +35,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>title</t>
   </si>
   <si>
-    <t>order_number</t>
-  </si>
-  <si>
-    <t>transaction_currency</t>
-  </si>
-  <si>
-    <t>discount_type</t>
-  </si>
-  <si>
-    <t>discount_value</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
-    <t>product_name</t>
-  </si>
-  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -68,9 +52,6 @@
     <t>tax</t>
   </si>
   <si>
-    <t>payment_method</t>
-  </si>
-  <si>
     <t>Kelsey Phillips</t>
   </si>
   <si>
@@ -89,43 +70,55 @@
     <t>Bank Transfer</t>
   </si>
   <si>
-    <t>exchange_rate</t>
-  </si>
-  <si>
-    <t>supplier_name</t>
-  </si>
-  <si>
     <t>Cash Purchase</t>
   </si>
   <si>
-    <t>purchase_date</t>
-  </si>
-  <si>
     <t>Inventory</t>
   </si>
   <si>
-    <t>payment_account</t>
-  </si>
-  <si>
-    <t>expense_account</t>
-  </si>
-  <si>
     <t>benificiary</t>
   </si>
   <si>
-    <t>project_code</t>
-  </si>
-  <si>
-    <t>project_task_code</t>
-  </si>
-  <si>
-    <t>cost_code</t>
+    <t>bill no</t>
+  </si>
+  <si>
+    <t>purchase date</t>
+  </si>
+  <si>
+    <t>vendor name</t>
+  </si>
+  <si>
+    <t>order number</t>
+  </si>
+  <si>
+    <t>transaction currency</t>
+  </si>
+  <si>
+    <t>exchange rate</t>
+  </si>
+  <si>
+    <t>discount type</t>
+  </si>
+  <si>
+    <t>discount value</t>
+  </si>
+  <si>
+    <t>product name</t>
+  </si>
+  <si>
+    <t>expense account</t>
+  </si>
+  <si>
+    <t>payment account</t>
+  </si>
+  <si>
+    <t>payment method</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,144 +430,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B2" s="1">
+        <v>45374</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="O2">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="P2" t="s">
         <v>8</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Q2" t="s">
         <v>9</v>
       </c>
-      <c r="S1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="R2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45374</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>27</v>
-      </c>
-      <c r="R2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>